<commit_message>
Start working on Branch Vivek
</commit_message>
<xml_diff>
--- a/sale system.xlsx
+++ b/sale system.xlsx
@@ -19,6 +19,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t xml:space="preserve">Product_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product_name</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -114,17 +125,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>